<commit_message>
Update readme and the Survey data
</commit_message>
<xml_diff>
--- a/Overall Data with Tagging Results.xlsx
+++ b/Overall Data with Tagging Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenhaowei/Desktop/EMP/jnose-results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenhaowei/Documents/research-related-data/Unit-Test-Empricial-Study-from-AAA-Perspective/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D246296-E647-5542-8B92-0F40095343B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA8F45E-4F21-0149-9CAF-F1FD9C997348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="-21960" windowWidth="30240" windowHeight="17680" activeTab="2" xr2:uid="{F4B7738A-8F1F-DA49-A4FA-7137EC39245F}"/>
+    <workbookView xWindow="-2820" yWindow="-24440" windowWidth="30240" windowHeight="17680" activeTab="1" xr2:uid="{F4B7738A-8F1F-DA49-A4FA-7137EC39245F}"/>
   </bookViews>
   <sheets>
     <sheet name="AAAVSJNOSE" sheetId="12" r:id="rId1"/>
@@ -3428,7 +3428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3616,6 +3616,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3959,7 +3961,7 @@
   <dimension ref="B2:N40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4024,7 +4026,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" s="53">
         <v>11</v>
@@ -5756,10 +5758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C597A31F-B7A6-6746-88B1-8FF32BF3804B}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5767,7 +5769,7 @@
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>886</v>
       </c>
@@ -5785,7 +5787,7 @@
       <c r="I1" s="92"/>
       <c r="J1" s="93"/>
     </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>889</v>
       </c>
@@ -5817,7 +5819,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
@@ -5857,8 +5859,36 @@
         <f>SUM(G3:I3)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f>SUM(B3:B5)</f>
+        <v>54</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:N3" si="0">SUM(C3:C5)</f>
+        <v>26</v>
+      </c>
+      <c r="N3">
+        <f>SUM(D3:D5)</f>
+        <v>18</v>
+      </c>
+      <c r="O3">
+        <f>SUM(E3:E5)</f>
+        <v>27</v>
+      </c>
+      <c r="Q3">
+        <f>SUM(G3:G5)</f>
+        <v>17</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:S3" si="1">SUM(H3:H5)</f>
+        <v>13</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
@@ -5879,7 +5909,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="17">
-        <f t="shared" ref="F4:F9" si="0">SUM(B4:E4)</f>
+        <f t="shared" ref="F4:F9" si="2">SUM(B4:E4)</f>
         <v>9</v>
       </c>
       <c r="G4" s="19">
@@ -5895,11 +5925,11 @@
         <v>10</v>
       </c>
       <c r="J4" s="20">
-        <f t="shared" ref="J4:J10" si="1">SUM(G4:I4)</f>
+        <f t="shared" ref="J4:J10" si="3">SUM(G4:I4)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>898</v>
       </c>
@@ -5920,7 +5950,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="G5" s="19">
@@ -5936,11 +5966,11 @@
         <v>0</v>
       </c>
       <c r="J5" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>4</v>
       </c>
@@ -5961,7 +5991,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G6" s="24">
@@ -5977,11 +6007,11 @@
         <v>3</v>
       </c>
       <c r="J6" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>3</v>
       </c>
@@ -6018,17 +6048,17 @@
         <v>0</v>
       </c>
       <c r="J7" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>899</v>
       </c>
       <c r="B8" s="17">
         <f>SUM(druid!G2:'druid'!G226)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="17">
         <f>SUM(dubbo!G$2:'dubbo'!G$78)</f>
@@ -6043,8 +6073,8 @@
         <v>1</v>
       </c>
       <c r="F8" s="17">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="G8" s="19">
         <f>SUM(archaius!G$2:G$101)</f>
@@ -6059,11 +6089,11 @@
         <v>0</v>
       </c>
       <c r="J8" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>900</v>
       </c>
@@ -6084,7 +6114,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="G9" s="19">
@@ -6100,11 +6130,11 @@
         <v>1</v>
       </c>
       <c r="J9" s="20">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>901</v>
       </c>
@@ -6138,12 +6168,12 @@
         <v>100</v>
       </c>
       <c r="J10" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>886</v>
       </c>
@@ -6161,7 +6191,7 @@
       <c r="I13" s="95"/>
       <c r="J13" s="96"/>
     </row>
-    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>889</v>
       </c>
@@ -6193,7 +6223,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>0</v>
       </c>
@@ -6202,72 +6232,101 @@
         <v>0.20444444444444446</v>
       </c>
       <c r="C15" s="32">
-        <f t="shared" ref="C15:J21" si="2">C3/C$10</f>
+        <f t="shared" ref="C15:J21" si="4">C3/C$10</f>
         <v>0.29870129870129869</v>
       </c>
       <c r="D15" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.36734693877551022</v>
       </c>
       <c r="E15" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="F15" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.23678160919540231</v>
       </c>
       <c r="G15" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.11</v>
       </c>
       <c r="H15" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="I15" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.06</v>
       </c>
       <c r="J15" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.09</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L15" s="98">
+        <f>SUM(B15:B17)</f>
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="M15" s="98">
+        <f t="shared" ref="M15:O15" si="5">SUM(C15:C17)</f>
+        <v>0.33766233766233766</v>
+      </c>
+      <c r="N15" s="98">
+        <f t="shared" si="5"/>
+        <v>0.36734693877551022</v>
+      </c>
+      <c r="O15" s="98">
+        <f t="shared" si="5"/>
+        <v>0.3214285714285714</v>
+      </c>
+      <c r="P15" s="98"/>
+      <c r="Q15" s="98">
+        <f t="shared" ref="Q15" si="6">SUM(G15:G17)</f>
+        <v>0.16999999999999998</v>
+      </c>
+      <c r="R15" s="98">
+        <f t="shared" ref="R15" si="7">SUM(H15:H17)</f>
+        <v>0.13</v>
+      </c>
+      <c r="S15" s="98">
+        <f t="shared" ref="S15" si="8">SUM(I15:I17)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="37">
-        <f t="shared" ref="B16:B21" si="3">B4/$B$10</f>
+        <f t="shared" ref="B16:B21" si="9">B4/$B$10</f>
         <v>4.4444444444444444E-3</v>
       </c>
       <c r="C16" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D16" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E16" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="F16" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.0689655172413793E-2</v>
       </c>
       <c r="G16" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="H16" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
       <c r="I16" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="J16" s="40">
@@ -6280,39 +6339,39 @@
         <v>898</v>
       </c>
       <c r="B17" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.111111111111111E-2</v>
       </c>
       <c r="C17" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.896103896103896E-2</v>
       </c>
       <c r="D17" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E17" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5714285714285712E-2</v>
       </c>
       <c r="F17" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.9885057471264367E-2</v>
       </c>
       <c r="G17" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
       <c r="H17" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I17" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J17" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
@@ -6321,39 +6380,39 @@
         <v>4</v>
       </c>
       <c r="B18" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C18" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.2987012987012988E-2</v>
       </c>
       <c r="D18" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E18" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="F18" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1494252873563218E-2</v>
       </c>
       <c r="G18" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H18" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I18" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
       <c r="J18" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
     </row>
@@ -6362,39 +6421,39 @@
         <v>3</v>
       </c>
       <c r="B19" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C19" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D19" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E19" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="F19" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.1954022988505746E-3</v>
       </c>
       <c r="G19" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H19" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I19" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J19" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -6403,39 +6462,39 @@
         <v>899</v>
       </c>
       <c r="B20" s="37">
-        <f t="shared" si="3"/>
-        <v>8.8888888888888889E-3</v>
+        <f t="shared" si="9"/>
+        <v>4.4444444444444444E-3</v>
       </c>
       <c r="C20" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D20" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E20" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1904761904761904E-2</v>
       </c>
       <c r="F20" s="37">
-        <f t="shared" si="2"/>
-        <v>6.8965517241379309E-3</v>
+        <f t="shared" si="4"/>
+        <v>4.5977011494252873E-3</v>
       </c>
       <c r="G20" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H20" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I20" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J20" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -6444,39 +6503,39 @@
         <v>900</v>
       </c>
       <c r="B21" s="42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.4444444444444444E-3</v>
       </c>
       <c r="C21" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.2987012987012988E-2</v>
       </c>
       <c r="D21" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E21" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F21" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.5977011494252873E-3</v>
       </c>
       <c r="G21" s="44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H21" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I21" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
       <c r="J21" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.3333333333333335E-3</v>
       </c>
     </row>
@@ -6488,6 +6547,7 @@
     <mergeCell ref="G13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6495,8 +6555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392EE06D-8B33-3C44-BE82-7A5C87338A99}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6751,7 +6811,7 @@
         <v>888</v>
       </c>
       <c r="B22" s="1" cm="1">
-        <f t="array" ref="B22">SUMPRODUCT((gson!B2:B101="")*(gson!C2:C101="")*(gson!D2:D101="")*(gson!E2:E101="")*(gson!F2:F101="")*(gson!H2:H101="")*(gson!I2:I101="")*(gson!J2:J101="")*(gson!K2:K101="")*(gson!L2:L101=""))+SUMPRODUCT((archaius!B2:B101="")*(archaius!C2:C101="")*(archaius!D2:D101="")*(archaius!E2:E101="")*(archaius!F2:F101="")*(archaius!H2:H101="")*(archaius!I2:I101="")*(archaius!J2:J101="")*(archaius!K2:K101="")*(archaius!L2:L101=""))+SUMPRODUCT(('mssql-jdbc'!B2:B101="")*('mssql-jdbc'!C2:C101="")*('mssql-jdbc'!D2:D101="")*('mssql-jdbc'!E2:E101="")*('mssql-jdbc'!F2:F101="")*('mssql-jdbc'!H2:H101="")*('mssql-jdbc'!I2:I101="")*('mssql-jdbc'!J2:J101="")*('mssql-jdbc'!K2:K101="")*('mssql-jdbc'!L2:L101=""))</f>
+        <f t="array" ref="B22">SUMPRODUCT((gson!B2:B101="")*(gson!C2:C101="")*(gson!D2:D101="")*(gson!E2:E101="")*(gson!F2:F101="")*(gson!G2:G101="")*(gson!H2:H101="")*(gson!I2:I101="")*(gson!J2:J101="")*(gson!K2:K101="")*(gson!L2:L101=""))+SUMPRODUCT((archaius!B2:B101="")*(archaius!C2:C101="")*(archaius!D2:D101="")*(archaius!E2:E101="")*(archaius!F2:F101="")*(archaius!G2:G101="")*(archaius!H2:H101="")*(archaius!I2:I101="")*(archaius!J2:J101="")*(archaius!K2:K101="")*(archaius!L2:L101=""))+SUMPRODUCT(('mssql-jdbc'!B2:B101="")*('mssql-jdbc'!C2:C101="")*('mssql-jdbc'!D2:D101="")*('mssql-jdbc'!E2:E101="")*('mssql-jdbc'!F2:F101="")*('mssql-jdbc'!G2:G101="")*('mssql-jdbc'!H2:H101="")*('mssql-jdbc'!I2:I101="")*('mssql-jdbc'!J2:J101="")*('mssql-jdbc'!K2:K101="")*('mssql-jdbc'!L2:L101=""))</f>
         <v>191</v>
       </c>
       <c r="C22" s="1">
@@ -6766,15 +6826,12 @@
         <v>887</v>
       </c>
       <c r="B23" s="1" cm="1">
-        <f t="array" ref="B23">SUMPRODUCT((druid!B2:B226="")*(druid!C2:C226="")*(druid!D2:D226="")*(druid!E2:E226="")*(druid!F2:F226="")*(druid!H2:H226="")*(druid!I2:I226="")*(druid!J2:J226="")*(druid!K2:K226="")*(druid!L2:L226=""))+
-SUMPRODUCT((dubbo!B2:B78="")*(dubbo!C2:C78="")*(dubbo!D2:D78="")*(dubbo!E2:E78="")*(dubbo!F2:F78="")*(dubbo!H2:H78="")*(dubbo!I2:I78="")*(dubbo!J2:J78="")*(dubbo!K2:K78="")*(dubbo!L2:L78=""))+
-SUMPRODUCT((accumulo!B2:B50="")*(accumulo!C2:C50="")*(accumulo!D2:D50="")*(accumulo!E2:E50="")*(accumulo!F2:F50="")*(accumulo!H2:H50="")*(accumulo!I2:I50="")*(accumulo!J2:J50="")*(accumulo!K2:K50="")*(accumulo!L2:L50=""))+
-SUMPRODUCT((cloudstack!B2:B85="")*(cloudstack!C2:C85="")*(cloudstack!D2:D85="")*(cloudstack!E2:E85="")*(cloudstack!F2:F85="")*(cloudstack!H2:H85="")*(cloudstack!I2:I85="")*(cloudstack!J2:J85="")*(cloudstack!K2:K85="")*(cloudstack!L2:L85=""))</f>
-        <v>271</v>
+        <f t="array" ref="B23">SUMPRODUCT((druid!B2:B226="")*(druid!C2:C226="")*(druid!D2:D226="")*(druid!E2:E226="")*(druid!F2:F226="")*(druid!G2:G226="")*(druid!H2:H226="")*(druid!I2:I226="")*(druid!J2:J226="")*(druid!K2:K226="")*(druid!L2:L226=""))+SUMPRODUCT((dubbo!B2:B78="")*(dubbo!C2:C78="")*(dubbo!D2:D78="")*(dubbo!E2:E78="")*(dubbo!F2:F78="")*(dubbo!G2:G78="")*(dubbo!H2:H78="")*(dubbo!I2:I78="")*(dubbo!J2:J78="")*(dubbo!K2:K78="")*(dubbo!L2:L78=""))+SUMPRODUCT((accumulo!B2:B50="")*(accumulo!C2:C50="")*(accumulo!D2:D50="")*(accumulo!E2:E50="")*(accumulo!F2:F50="")*(accumulo!G2:G50="")*(accumulo!H2:H50="")*(accumulo!I2:I50="")*(accumulo!J2:J50="")*(accumulo!K2:K50="")*(accumulo!L2:L50=""))+SUMPRODUCT((cloudstack!B2:B85="")*(cloudstack!C2:C85="")*(cloudstack!D2:D85="")*(cloudstack!E2:E85="")*(cloudstack!F2:F85="")*(cloudstack!G2:G85="")*(cloudstack!H2:H85="")*(cloudstack!I2:I85="")*(cloudstack!J2:J85="")*(cloudstack!K2:K85="")*(cloudstack!L2:L85=""))</f>
+        <v>269</v>
       </c>
       <c r="C23" s="1">
         <f>SUM(B28:E28)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -6785,11 +6842,11 @@
       </c>
       <c r="B24" s="1">
         <f>B23+B22</f>
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C24" s="1">
         <f>C22+C23</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -6853,7 +6910,7 @@
       </c>
       <c r="D28" s="1">
         <f>SUM(druid!G2:G226)+SUM(dubbo!G2:G78)+SUM(accumulo!G2:G50)+SUM(cloudstack!G2:G85)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28" s="1">
         <f>SUM(druid!H2:H226)+SUM(dubbo!H2:H78)+SUM(accumulo!H2:H50)+SUM(cloudstack!H2:H85)</f>
@@ -6874,7 +6931,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="1"/>
@@ -6978,13 +7035,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF17DF3-05C6-5642-81E7-149383305302}">
   <dimension ref="A1:V226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="115.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
     <col min="9" max="9" width="28.1640625" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" customWidth="1"/>
     <col min="11" max="11" width="16.1640625" customWidth="1"/>
@@ -8132,14 +8190,11 @@
         <v>883</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+    <row r="111" spans="1:22" s="97" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="97" t="s">
         <v>455</v>
       </c>
-      <c r="G111">
-        <v>1</v>
-      </c>
-      <c r="M111" t="s">
+      <c r="M111" s="97" t="s">
         <v>12</v>
       </c>
     </row>
@@ -9324,7 +9379,7 @@
   <dimension ref="A1:V78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10239,7 +10294,7 @@
   <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11153,7 +11208,7 @@
   <dimension ref="A1:V85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12118,7 +12173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76B9D9-487E-6440-B83E-8A62C900A02D}">
   <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>

</xml_diff>